<commit_message>
Changes to be committed: 	modified:   Codes/Plot graph 	modified:   Extracted Data/VRU Headform - Color-wise graph/2020_cars_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graph/2022_cars_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graph/2023_cars_combined.xlsx 	modified:   Extracted Data/VRU Headform - Color-wise graph/2024_cars_combined.xlsx
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform - Color-wise graph/2020_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform - Color-wise graph/2020_cars_combined.xlsx
@@ -7,7 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Graphs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Default green" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Green" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Yellow" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Orange" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Brown" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Red" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Default Red" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Blue" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -151,6 +158,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -161,11 +173,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -176,6 +188,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -186,11 +203,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -201,6 +218,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -211,11 +233,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -226,6 +248,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -236,11 +263,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -251,6 +278,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -261,11 +293,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -276,6 +308,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -286,11 +323,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -301,6 +338,11 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -311,11 +353,11 @@
     <ext cx="6096000" cy="4572000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="8" name="Image 8" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip cstate="print" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -629,4 +671,137 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>